<commit_message>
updates and add conclusion
</commit_message>
<xml_diff>
--- a/plotting/calculator.xlsx
+++ b/plotting/calculator.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>Code version</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,6 +127,10 @@
   </si>
   <si>
     <t>SpeedUp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>avx_opcount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -609,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -620,7 +624,9 @@
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.875" style="2" customWidth="1"/>
     <col min="8" max="8" width="18" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="2"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -664,6 +670,9 @@
         <v>17</v>
       </c>
       <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
         <v>19</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -1271,37 +1280,34 @@
         <v>192</v>
       </c>
       <c r="D26">
-        <v>2794924</v>
-      </c>
-      <c r="E26">
-        <v>2972306</v>
-      </c>
-      <c r="F26">
-        <v>5140</v>
+        <v>2359028</v>
       </c>
       <c r="G26" s="5">
-        <f>K26+L26+M26+N26</f>
-        <v>1585686</v>
+        <f>K26+L26+M26+N26+O26</f>
+        <v>34322347</v>
       </c>
       <c r="H26" s="6">
         <f>G26/D26</f>
-        <v>0.56734494390545143</v>
+        <v>14.54935973629817</v>
       </c>
       <c r="K26">
-        <v>426826</v>
+        <v>9254482</v>
       </c>
       <c r="L26">
-        <v>1084519</v>
+        <v>19958851</v>
       </c>
       <c r="M26">
-        <v>69203</v>
+        <v>3518120</v>
       </c>
       <c r="N26">
-        <v>5138</v>
+        <v>1344500</v>
+      </c>
+      <c r="O26">
+        <v>246394</v>
       </c>
       <c r="P26" s="5">
         <f>D2/D26</f>
-        <v>2652.8951080601832</v>
+        <v>3143.0912252843118</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1312,37 +1318,34 @@
         <v>224</v>
       </c>
       <c r="D27">
-        <v>3480558</v>
-      </c>
-      <c r="E27">
-        <v>5789337</v>
-      </c>
-      <c r="F27">
-        <v>7515</v>
-      </c>
-      <c r="G27" s="2">
-        <f>K27+L27+M27+N27</f>
-        <v>3035341</v>
+        <v>2604626</v>
+      </c>
+      <c r="G27" s="5">
+        <f>K27+L27+M27+N27+O27</f>
+        <v>47759630</v>
       </c>
       <c r="H27" s="1">
         <f>G27/D27</f>
-        <v>0.87208459103396641</v>
+        <v>18.336463661193584</v>
       </c>
       <c r="K27">
-        <v>863450</v>
+        <v>13960000</v>
       </c>
       <c r="L27">
-        <v>2052642</v>
+        <v>25709593</v>
       </c>
       <c r="M27">
-        <v>111736</v>
+        <v>5851018</v>
       </c>
       <c r="N27">
-        <v>7513</v>
+        <v>1946000</v>
+      </c>
+      <c r="O27">
+        <v>293019</v>
       </c>
       <c r="P27" s="2">
         <f>D3/D27</f>
-        <v>3628.6644115684899</v>
+        <v>4848.9790653245418</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1353,37 +1356,34 @@
         <v>256</v>
       </c>
       <c r="D28">
-        <v>3899886</v>
-      </c>
-      <c r="E28">
-        <v>6199073</v>
-      </c>
-      <c r="F28">
-        <v>7822</v>
-      </c>
-      <c r="G28" s="2">
-        <f>K28+L28+M28+N28</f>
-        <v>3257705</v>
+        <v>3179679</v>
+      </c>
+      <c r="G28" s="5">
+        <f>K28+L28+M28+N28+O28</f>
+        <v>55548811</v>
       </c>
       <c r="H28" s="1">
         <f>G28/D28</f>
-        <v>0.83533339179658073</v>
+        <v>17.469943035130274</v>
       </c>
       <c r="K28">
-        <v>922903</v>
+        <v>15843826</v>
       </c>
       <c r="L28">
-        <v>2208648</v>
+        <v>31034535</v>
       </c>
       <c r="M28">
-        <v>118334</v>
+        <v>6012434</v>
       </c>
       <c r="N28">
-        <v>7820</v>
+        <v>2334000</v>
+      </c>
+      <c r="O28">
+        <v>324016</v>
       </c>
       <c r="P28" s="2">
         <f>D4/D28</f>
-        <v>4121.6421259493227</v>
+        <v>5055.2066494762521</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1394,37 +1394,34 @@
         <v>384</v>
       </c>
       <c r="D29">
-        <v>9863363</v>
-      </c>
-      <c r="E29">
-        <v>19250012</v>
-      </c>
-      <c r="F29">
-        <v>14815</v>
-      </c>
-      <c r="G29" s="2">
-        <f>K29+L29+M29+N29</f>
-        <v>9848295</v>
+        <v>7252693</v>
+      </c>
+      <c r="G29" s="5">
+        <f>K29+L29+M29+N29+O29</f>
+        <v>113896159</v>
       </c>
       <c r="H29" s="1">
         <f>G29/D29</f>
-        <v>0.99847232632520977</v>
+        <v>15.703981817512474</v>
       </c>
       <c r="K29">
-        <v>2937601</v>
+        <v>35166241</v>
       </c>
       <c r="L29">
-        <v>6635143</v>
+        <v>61496918</v>
       </c>
       <c r="M29">
-        <v>260738</v>
+        <v>13041998</v>
       </c>
       <c r="N29">
-        <v>14813</v>
+        <v>3701500</v>
+      </c>
+      <c r="O29">
+        <v>489502</v>
       </c>
       <c r="P29" s="2">
         <f>D5/D29</f>
-        <v>5844.5757423710347</v>
+        <v>7948.3816739520062</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1435,37 +1432,34 @@
         <v>521</v>
       </c>
       <c r="D30">
-        <v>24905849</v>
-      </c>
-      <c r="E30">
-        <v>56765947</v>
-      </c>
-      <c r="F30">
-        <v>28853</v>
-      </c>
-      <c r="G30" s="2">
-        <f>K30+L30+M30+N30</f>
-        <v>28765815</v>
+        <v>15988047</v>
+      </c>
+      <c r="G30" s="5">
+        <f>K30+L30+M30+N30+O30</f>
+        <v>214115218</v>
       </c>
       <c r="H30" s="1">
         <f>G30/D30</f>
-        <v>1.1549823095771599</v>
+        <v>13.392205939849939</v>
       </c>
       <c r="K30">
-        <v>8946918</v>
+        <v>72765931</v>
       </c>
       <c r="L30">
-        <v>19255128</v>
+        <v>105889794</v>
       </c>
       <c r="M30">
-        <v>534966</v>
+        <v>27779438</v>
       </c>
       <c r="N30">
-        <v>28803</v>
+        <v>6971000</v>
+      </c>
+      <c r="O30">
+        <v>709055</v>
       </c>
       <c r="P30" s="2">
         <f>D6/D30</f>
-        <v>5716.1020870639668</v>
+        <v>8904.4256280332429</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="14.25" thickBot="1">
@@ -1672,19 +1666,19 @@
         <v>23</v>
       </c>
       <c r="B55">
-        <v>2785452</v>
+        <v>1396200</v>
       </c>
       <c r="C55">
-        <v>2523639</v>
+        <v>1637724</v>
       </c>
       <c r="D55">
-        <v>2773645</v>
+        <v>1793954</v>
       </c>
       <c r="E55">
-        <v>6012075</v>
+        <v>4078117</v>
       </c>
       <c r="F55">
-        <v>13953763</v>
+        <v>8865370</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -1692,19 +1686,19 @@
         <v>24</v>
       </c>
       <c r="B56">
-        <v>1846116</v>
+        <v>1987830</v>
       </c>
       <c r="C56">
-        <v>2351263</v>
+        <v>2570753</v>
       </c>
       <c r="D56">
-        <v>3043013</v>
+        <v>3187398</v>
       </c>
       <c r="E56">
-        <v>5688408</v>
+        <v>6069194</v>
       </c>
       <c r="F56">
-        <v>12652617</v>
+        <v>13571951</v>
       </c>
     </row>
     <row r="57" spans="1:16" s="2" customFormat="1">
@@ -1713,28 +1707,28 @@
       </c>
       <c r="B57" s="2">
         <f>B56/B55</f>
-        <v>0.66277071010378208</v>
+        <v>1.4237430167597764</v>
       </c>
       <c r="C57" s="2">
         <f>C56/C55</f>
-        <v>0.93169546040459827</v>
+        <v>1.5697107693359809</v>
       </c>
       <c r="D57" s="2">
         <f>D56/D55</f>
-        <v>1.0971169706289017</v>
+        <v>1.7767445542081903</v>
       </c>
       <c r="E57" s="2">
         <f>E56/E55</f>
-        <v>0.9461638452614114</v>
+        <v>1.4882343983755248</v>
       </c>
       <c r="F57" s="2">
         <f>F56/F55</f>
-        <v>0.90675303858894551</v>
+        <v>1.5308950444256697</v>
       </c>
     </row>
     <row r="59" spans="1:16">
       <c r="A59">
-        <v>101010</v>
+        <v>100000</v>
       </c>
       <c r="B59">
         <v>192</v>
@@ -1757,19 +1751,19 @@
         <v>23</v>
       </c>
       <c r="B60">
-        <v>2787918</v>
+        <v>975663</v>
       </c>
       <c r="C60">
-        <v>2339580</v>
+        <v>986119</v>
       </c>
       <c r="D60">
-        <v>2542611</v>
+        <v>1088488</v>
       </c>
       <c r="E60">
-        <v>5484323</v>
+        <v>2379518</v>
       </c>
       <c r="F60">
-        <v>12420764</v>
+        <v>5350095</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -1777,19 +1771,19 @@
         <v>24</v>
       </c>
       <c r="B61">
-        <v>1745411</v>
+        <v>1756744</v>
       </c>
       <c r="C61">
-        <v>2269896</v>
+        <v>2148763</v>
       </c>
       <c r="D61">
-        <v>2810164</v>
+        <v>2617051</v>
       </c>
       <c r="E61">
-        <v>5685599</v>
+        <v>5218790</v>
       </c>
       <c r="F61">
-        <v>12341146</v>
+        <v>11295713</v>
       </c>
     </row>
     <row r="62" spans="1:16" s="2" customFormat="1">
@@ -1798,28 +1792,28 @@
       </c>
       <c r="B62" s="2">
         <f>B61/B60</f>
-        <v>0.62606253125091915</v>
+        <v>1.800564334201461</v>
       </c>
       <c r="C62" s="2">
         <f>C61/C60</f>
-        <v>0.97021516682481468</v>
+        <v>2.1790098355269496</v>
       </c>
       <c r="D62" s="2">
         <f>D61/D60</f>
-        <v>1.1052276577109121</v>
+        <v>2.4042993583760226</v>
       </c>
       <c r="E62" s="2">
         <f>E61/E60</f>
-        <v>1.0367002454085947</v>
+        <v>2.193213079287486</v>
       </c>
       <c r="F62" s="2">
         <f>F61/F60</f>
-        <v>0.99358992731848061</v>
+        <v>2.1113107337346344</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65">
-        <v>100000</v>
+        <v>101010</v>
       </c>
       <c r="B65">
         <v>192</v>
@@ -1842,19 +1836,19 @@
         <v>23</v>
       </c>
       <c r="B66">
-        <v>2585513</v>
+        <v>1038435</v>
       </c>
       <c r="C66">
-        <v>2132071</v>
+        <v>1148436</v>
       </c>
       <c r="D66">
-        <v>2296595</v>
+        <v>1315052</v>
       </c>
       <c r="E66">
-        <v>4812421</v>
+        <v>2800620</v>
       </c>
       <c r="F66">
-        <v>10906483</v>
+        <v>6149847</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1862,19 +1856,19 @@
         <v>24</v>
       </c>
       <c r="B67">
-        <v>1598446</v>
+        <v>1812611</v>
       </c>
       <c r="C67">
-        <v>2095973</v>
+        <v>2232083</v>
       </c>
       <c r="D67">
-        <v>2629027</v>
+        <v>2838611</v>
       </c>
       <c r="E67">
-        <v>5258271</v>
+        <v>5673912</v>
       </c>
       <c r="F67">
-        <v>11465776</v>
+        <v>12057395</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="2" customFormat="1">
@@ -1883,23 +1877,23 @@
       </c>
       <c r="B68" s="2">
         <f>B67/B66</f>
-        <v>0.6182316623432178</v>
+        <v>1.7455218670403059</v>
       </c>
       <c r="C68" s="2">
         <f>C67/C66</f>
-        <v>0.98306904413595986</v>
+        <v>1.9435850147504954</v>
       </c>
       <c r="D68" s="2">
         <f>D67/D66</f>
-        <v>1.1447499450273122</v>
+        <v>2.1585541864504219</v>
       </c>
       <c r="E68" s="2">
         <f>E67/E66</f>
-        <v>1.092645676677082</v>
+        <v>2.0259485399661505</v>
       </c>
       <c r="F68" s="2">
         <f>F67/F66</f>
-        <v>1.0512807840987788</v>
+        <v>1.9606008084428768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update plots and report
</commit_message>
<xml_diff>
--- a/plotting/calculator.xlsx
+++ b/plotting/calculator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="14190" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1284,23 +1284,23 @@
       </c>
       <c r="G26" s="5">
         <f>K26+L26+M26+N26+O26</f>
-        <v>34322347</v>
+        <v>590975</v>
       </c>
       <c r="H26" s="6">
         <f>G26/D26</f>
-        <v>14.54935973629817</v>
+        <v>0.25051631434641725</v>
       </c>
       <c r="K26">
-        <v>9254482</v>
+        <v>92322</v>
       </c>
       <c r="L26">
-        <v>19958851</v>
+        <v>199576</v>
       </c>
       <c r="M26">
-        <v>3518120</v>
+        <v>52683</v>
       </c>
       <c r="N26">
-        <v>1344500</v>
+        <v>0</v>
       </c>
       <c r="O26">
         <v>246394</v>
@@ -1322,23 +1322,23 @@
       </c>
       <c r="G27" s="5">
         <f>K27+L27+M27+N27+O27</f>
-        <v>47759630</v>
+        <v>770052</v>
       </c>
       <c r="H27" s="1">
         <f>G27/D27</f>
-        <v>18.336463661193584</v>
+        <v>0.2956478204548369</v>
       </c>
       <c r="K27">
-        <v>13960000</v>
+        <v>139226</v>
       </c>
       <c r="L27">
-        <v>25709593</v>
+        <v>256289</v>
       </c>
       <c r="M27">
-        <v>5851018</v>
+        <v>81518</v>
       </c>
       <c r="N27">
-        <v>1946000</v>
+        <v>0</v>
       </c>
       <c r="O27">
         <v>293019</v>
@@ -1360,23 +1360,23 @@
       </c>
       <c r="G28" s="5">
         <f>K28+L28+M28+N28+O28</f>
-        <v>55548811</v>
+        <v>882158</v>
       </c>
       <c r="H28" s="1">
         <f>G28/D28</f>
-        <v>17.469943035130274</v>
+        <v>0.27743618145102067</v>
       </c>
       <c r="K28">
-        <v>15843826</v>
+        <v>158049</v>
       </c>
       <c r="L28">
-        <v>31034535</v>
+        <v>310193</v>
       </c>
       <c r="M28">
-        <v>6012434</v>
+        <v>89900</v>
       </c>
       <c r="N28">
-        <v>2334000</v>
+        <v>0</v>
       </c>
       <c r="O28">
         <v>324016</v>
@@ -1398,23 +1398,23 @@
       </c>
       <c r="G29" s="5">
         <f>K29+L29+M29+N29+O29</f>
-        <v>113896159</v>
+        <v>1652927</v>
       </c>
       <c r="H29" s="1">
         <f>G29/D29</f>
-        <v>15.703981817512474</v>
+        <v>0.22790527601264798</v>
       </c>
       <c r="K29">
-        <v>35166241</v>
+        <v>350800</v>
       </c>
       <c r="L29">
-        <v>61496918</v>
+        <v>619485</v>
       </c>
       <c r="M29">
-        <v>13041998</v>
+        <v>193140</v>
       </c>
       <c r="N29">
-        <v>3701500</v>
+        <v>0</v>
       </c>
       <c r="O29">
         <v>489502</v>
@@ -1436,23 +1436,23 @@
       </c>
       <c r="G30" s="5">
         <f>K30+L30+M30+N30+O30</f>
-        <v>214115218</v>
+        <v>2897612</v>
       </c>
       <c r="H30" s="1">
         <f>G30/D30</f>
-        <v>13.392205939849939</v>
+        <v>0.1812361447273704</v>
       </c>
       <c r="K30">
-        <v>72765931</v>
+        <v>725781</v>
       </c>
       <c r="L30">
-        <v>105889794</v>
+        <v>1067380</v>
       </c>
       <c r="M30">
-        <v>27779438</v>
+        <v>395396</v>
       </c>
       <c r="N30">
-        <v>6971000</v>
+        <v>0</v>
       </c>
       <c r="O30">
         <v>709055</v>

</xml_diff>

<commit_message>
Unified the color of the lines
</commit_message>
<xml_diff>
--- a/plotting/calculator.xlsx
+++ b/plotting/calculator.xlsx
@@ -614,7 +614,7 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="P26" sqref="P26:P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1284,17 +1284,17 @@
       </c>
       <c r="G26" s="5">
         <f>K26+L26+M26+N26+O26</f>
-        <v>590975</v>
+        <v>1514359</v>
       </c>
       <c r="H26" s="6">
         <f>G26/D26</f>
-        <v>0.25051631434641725</v>
+        <v>0.64194193540729483</v>
       </c>
       <c r="K26">
-        <v>92322</v>
+        <v>344154</v>
       </c>
       <c r="L26">
-        <v>199576</v>
+        <v>871128</v>
       </c>
       <c r="M26">
         <v>52683</v>
@@ -1322,17 +1322,17 @@
       </c>
       <c r="G27" s="5">
         <f>K27+L27+M27+N27+O27</f>
-        <v>770052</v>
+        <v>2658260</v>
       </c>
       <c r="H27" s="1">
         <f>G27/D27</f>
-        <v>0.2956478204548369</v>
+        <v>1.0205918239317275</v>
       </c>
       <c r="K27">
-        <v>139226</v>
+        <v>678714</v>
       </c>
       <c r="L27">
-        <v>256289</v>
+        <v>1605009</v>
       </c>
       <c r="M27">
         <v>81518</v>
@@ -1360,17 +1360,17 @@
       </c>
       <c r="G28" s="5">
         <f>K28+L28+M28+N28+O28</f>
-        <v>882158</v>
+        <v>2921776</v>
       </c>
       <c r="H28" s="1">
         <f>G28/D28</f>
-        <v>0.27743618145102067</v>
+        <v>0.91889024017833243</v>
       </c>
       <c r="K28">
-        <v>158049</v>
+        <v>740797</v>
       </c>
       <c r="L28">
-        <v>310193</v>
+        <v>1767063</v>
       </c>
       <c r="M28">
         <v>89900</v>
@@ -1398,17 +1398,17 @@
       </c>
       <c r="G29" s="5">
         <f>K29+L29+M29+N29+O29</f>
-        <v>1652927</v>
+        <v>8330147</v>
       </c>
       <c r="H29" s="1">
         <f>G29/D29</f>
-        <v>0.22790527601264798</v>
+        <v>1.148559162782707</v>
       </c>
       <c r="K29">
-        <v>350800</v>
+        <v>2353966</v>
       </c>
       <c r="L29">
-        <v>619485</v>
+        <v>5293539</v>
       </c>
       <c r="M29">
         <v>193140</v>
@@ -1436,17 +1436,17 @@
       </c>
       <c r="G30" s="5">
         <f>K30+L30+M30+N30+O30</f>
-        <v>2897612</v>
+        <v>23641834</v>
       </c>
       <c r="H30" s="1">
         <f>G30/D30</f>
-        <v>0.1812361447273704</v>
+        <v>1.4787193207525597</v>
       </c>
       <c r="K30">
-        <v>725781</v>
+        <v>7163643</v>
       </c>
       <c r="L30">
-        <v>1067380</v>
+        <v>15373740</v>
       </c>
       <c r="M30">
         <v>395396</v>

</xml_diff>